<commit_message>
0.2.2: Implement ignoreImport option. * not implement yet java specific import section.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CC7B52-7EB1-7E49-A438-1C8B69930B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E898D8-08AA-0E4B-90FE-EA349D6E3029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16360" yWindow="2140" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -611,6 +611,23 @@
     </rPh>
     <rPh sb="23" eb="25">
       <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ignoreImport</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Java向け以外のインポートを無視します。</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ムケ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">イガイノ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">ムシシマス。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1628,7 +1645,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1672,7 +1689,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1697,10 +1714,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1905,7 +1922,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A35" si="0">A15+1</f>
+        <f t="shared" ref="A16:A36" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -2344,16 +2361,27 @@
       <c r="J35" s="60"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="27"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
+      <c r="A36" s="27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="32"/>
+      <c r="E36" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="60"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="27"/>
@@ -2393,8 +2421,8 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
       <c r="D40" s="29"/>
       <c r="E40" s="30"/>
       <c r="F40" s="31"/>
@@ -2429,8 +2457,8 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="27"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31"/>
@@ -2488,7 +2516,7 @@
       <c r="J47" s="32"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="34"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
       <c r="D48" s="29"/>
@@ -2512,16 +2540,28 @@
       <c r="J49" s="32"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="35"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="40"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="32"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="35"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2539,17 +2579,17 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F66" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C24 C28:C50" xr:uid="{19DD6A3C-A5DD-0544-96F2-8B8D8DA816D2}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C24 C28:C51" xr:uid="{19DD6A3C-A5DD-0544-96F2-8B8D8DA816D2}">
       <formula1>型リスト</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D16 D36:D50 D18:D24 D28:D33" xr:uid="{78445AB0-9400-7A43-BA63-9EA5A5ED49CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D16 D37:D51 D18:D24 D28:D33" xr:uid="{78445AB0-9400-7A43-BA63-9EA5A5ED49CC}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D17 D34:D35 D25:D27" xr:uid="{0BA8ED15-AA00-B44F-A492-05A5F7CCEDA2}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D17 D25:D27 D34:D36" xr:uid="{0BA8ED15-AA00-B44F-A492-05A5F7CCEDA2}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.2.4: telegramsOnly option is implemented.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E898D8-08AA-0E4B-90FE-EA349D6E3029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6CF5A0-0CEE-F443-A519-B84D16E5591F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16360" yWindow="2140" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -628,6 +628,32 @@
     </rPh>
     <rPh sb="15" eb="17">
       <t xml:space="preserve">ムシシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>telegramsOnly</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>電文のみを生成し、電文処理は生成しません。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ノミヲ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ショリハ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">セイセイシマセン。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1645,7 +1671,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1689,7 +1715,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1717,7 +1743,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1922,7 +1948,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A36" si="0">A15+1</f>
+        <f t="shared" ref="A16:A37" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -2384,12 +2410,23 @@
       <c r="J36" s="60"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="27"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
+      <c r="A37" s="27">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>85</v>
+      </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
       <c r="I37" s="31"/>

</xml_diff>